<commit_message>
Fix to allow the user to enter subjects name by parts when these appear by parts in GEO record.
</commit_message>
<xml_diff>
--- a/GEO_list.xlsx
+++ b/GEO_list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,9 +16,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1522" uniqueCount="631">
-  <si>
-    <t>GSE52428</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1522" uniqueCount="630">
+  <si>
+    <t>GSE46298</t>
   </si>
   <si>
     <t>0,0.1,0.5,1,2,2.5,4,5,6,7,9,10,13,20,30,50,59,109,150,241</t>
@@ -63,7 +63,7 @@
     <t>SERIES</t>
   </si>
   <si>
-    <t>Total RNA from unfixed staged eggs at sequential (2h, 4h, 6h, 7h, 8h, 10h, 13h, 16h, 19h,  22h, 25h, 28.5h, 31h, 34h, 37h, 40h, 43h, 46h, 49h, 52h) time points was purified initially by Trizol (Invitrogen) and then further by RNAeasy (Qiagen) kit. </t>
+    <t>Total RNA from unfixed staged eggs at sequential (2h, 4h, 6h, 7h, 8h, 10h, 13h, 16h, 19h,  22h, 25h, 28.5h, 31h, 34h, 37h, 40h, 43h, 46h, 49h, 52h) time points was purified initially by Trizol (Invitrogen) and then further by RNAeasy (Qiagen) kit.</t>
   </si>
   <si>
     <t>0,20,40,60,80,100,120,140,160,180,200,220,240,260,280,300,320,340,360</t>
@@ -112,7 +112,7 @@
   </si>
   <si>
     <r>
-      <t>L1 Cells were treated either with 0.5% DMSO or 2 </t>
+      <t>L1 Cells were treated either with 0.5% DMSO or 2</t>
     </r>
     <r>
       <rPr>
@@ -120,6 +120,7 @@
         <color rgb="FF000000"/>
         <rFont val="WenQuanYi Zen Hei Sharp"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>碌</t>
     </r>
@@ -131,7 +132,7 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t>M of prieurianin for the following times: 0, 0.25, 0.5,1, 2, 3, 5, 9, 12, 15, 24, 36, 48, 96, 144, 192, 240, and 288 hrs, and then total RNA was purified at the indicated times using the RNeasy Mini kit according to the manufacturer�s instructions. </t>
+      <t>M of prieurianin for the following times: 0, 0.25, 0.5,1, 2, 3, 5, 9, 12, 15, 24, 36, 48, 96, 144, 192, 240, and 288 hrs, and then total RNA was purified at the indicated times using the RNeasy Mini kit according to the manufacturer�s instructions.</t>
     </r>
   </si>
   <si>
@@ -270,7 +271,7 @@
     <t>12,18,24,30,33,39,42,45,51,57,60,69,72,96,120,144</t>
   </si>
   <si>
-    <t>16 time points were designed at 12, 18, 24, 30, 33, 39, 42, 45, 51, 57, 60, 69, 72, 96, 120, and 144 hours. </t>
+    <t>16 time points were designed at 12, 18, 24, 30, 33, 39, 42, 45, 51, 57, 60, 69, 72, 96, 120, and 144 hours.</t>
   </si>
   <si>
     <t>0,1,2,3,6,7,10,21,24,25,30,45,48,55,90,180</t>
@@ -318,13 +319,13 @@
     <t>0,2,4,6,8,10,12,15,20,25,30,35,40,45,50,60</t>
   </si>
   <si>
-    <t> Targets were obtained from 16 time points: 0, 2, 4, 6, 8, 10, 12, 15, 20, 25, 30, 35, 40, 45, 50, 60 minutes after transcription inhibition. </t>
+    <t>Targets were obtained from 16 time points: 0, 2, 4, 6, 8, 10, 12, 15, 20, 25, 30, 35, 40, 45, 50, 60 minutes after transcription inhibition.</t>
   </si>
   <si>
     <t>0.25,0.5,0.75,1,2,4,5,5.5,6,7,8,12,18,30,48,72</t>
   </si>
   <si>
-    <t>The time points were: 0.25, 0.5, 0.75, 1, 2, 4, 5, 5.5, 6, 7, 8, 12, 18, 30, 48 and, 72 hours after dosing. </t>
+    <t>The time points were: 0.25, 0.5, 0.75, 1, 2, 4, 5, 5.5, 6, 7, 8, 12, 18, 30, 48 and, 72 hours after dosing.</t>
   </si>
   <si>
     <t>1,6,8,9,10,12,13,14,15,16,17,19,20,26,29</t>
@@ -462,7 +463,7 @@
     <t>0,1,3,5,7,10,15,20,30,40,50,60,80,120</t>
   </si>
   <si>
-    <t>Gene expression was measured at fourteen time intervals (0, 1, 3, 5, 7, 10, 15, 20, 30, 40, 50, 60, 80 and 120 min) during phage infection according to proposed loop. </t>
+    <t>Gene expression was measured at fourteen time intervals (0, 1, 3, 5, 7, 10, 15, 20, 30, 40, 50, 60, 80 and 120 min) during phage infection according to proposed loop.</t>
   </si>
   <si>
     <t>0,2,15,30,45,60,75,90,105,120,135,150,165,180</t>
@@ -507,7 +508,7 @@
     <t>0,5,10,15,20,25,30,35,40,50,60,70,80,90</t>
   </si>
   <si>
-    <t>In total, 14 samples were harvested at time points 0, 5, 10, 15, 20, 25, 30, 35, 40, 50, 60, 70, 80 and 90 min after switching from aerobic to microaerobic condition. </t>
+    <t>In total, 14 samples were harvested at time points 0, 5, 10, 15, 20, 25, 30, 35, 40, 50, 60, 70, 80 and 90 min after switching from aerobic to microaerobic condition.</t>
   </si>
   <si>
     <t>0,1,1.5,2,2.5,3,3.5,4,4.5,5,5.5,6,7,8</t>
@@ -522,22 +523,22 @@
     <t>0,1,2,3,4,5,6,7,8,9,11,13,15,17</t>
   </si>
   <si>
-    <t>Samples were harvested at 24 hour intervals on days 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 11, 13, 15, and 17. </t>
-  </si>
-  <si>
-    <t>Samples were harvested at 24 hour intervals on days 0,1, 2, 3, 4, 5, 6, 7, 8, 9, 11, 13, 15, and 17. </t>
+    <t>Samples were harvested at 24 hour intervals on days 0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 11, 13, 15, and 17.</t>
+  </si>
+  <si>
+    <t>Samples were harvested at 24 hour intervals on days 0,1, 2, 3, 4, 5, 6, 7, 8, 9, 11, 13, 15, and 17.</t>
   </si>
   <si>
     <t>0,0.04,0.08,0.13,0.19,0.25,0.38,0.5,1,2,3,4,5,6</t>
   </si>
   <si>
-    <t>At time zero (generation 0) the saprge gas was switched from air to O2-free N2 and samples were harvested after 0 (aerobic control), 0.04, 0.08, 0.13, 0.19, 0.25, 0.38, 0.5, 1, 2, 3, 4, 5 and 6 generations of anaerobic growth. </t>
+    <t>At time zero (generation 0) the saprge gas was switched from air to O2-free N2 and samples were harvested after 0 (aerobic control), 0.04, 0.08, 0.13, 0.19, 0.25, 0.38, 0.5, 1, 2, 3, 4, 5 and 6 generations of anaerobic growth.</t>
   </si>
   <si>
     <t>15,17,19,21,23,25,28,31,32,35,37,38,41,45</t>
   </si>
   <si>
-    <t>The time-course study involved analysis of 14 samples (15h, 17h, 19h, 21h, 23h, 25h, 28h, 31h, 32h, 35h, 37h, 38h, 41h, 45h). </t>
+    <t>The time-course study involved analysis of 14 samples (15h, 17h, 19h, 21h, 23h, 25h, 28h, 31h, 32h, 35h, 37h, 38h, 41h, 45h).</t>
   </si>
   <si>
     <t>0,4,6,10,12,14,18,27,31,33,37,45,50</t>
@@ -576,7 +577,7 @@
     <t>14,16,18,20,22,24,26,28,30,32,34,37,39</t>
   </si>
   <si>
-    <t>The time-course study involved analysis of 13 samples (14h, 16h, 18h, 20h, 22h, 24h, 26h, 28h, 30h, 32h, 34h, 37h, 39h). </t>
+    <t>The time-course study involved analysis of 13 samples (14h, 16h, 18h, 20h, 22h, 24h, 26h, 28h, 30h, 32h, 34h, 37h, 39h).</t>
   </si>
   <si>
     <t>-8,0,3,6,7,8,9,10,13,14,16,17,22</t>
@@ -648,31 +649,31 @@
     <t>1,2,3,4,5,6,7,9,10,11,12,13,14</t>
   </si>
   <si>
-    <t>Blood, saliva, and throat swabs were collected on days 0, 1, 2, 4, 7, 9, 16, 23, 32, 45, 58, 72, and 86. </t>
+    <t>Blood, saliva, and throat swabs were collected on days 0, 1, 2, 4, 7, 9, 16, 23, 32, 45, 58, 72, and 86.</t>
   </si>
   <si>
     <t>3,5,7,9,11,12,13,14,15,16,17,18,19</t>
   </si>
   <si>
-    <t> Except for the seven naive animals from the baseline group, nine animals (seven from the EAE and two from the control group) were sacrificed (at the same time of the day) at each of 13 time points after immunization, which are detailed as days 3, 5, 7, 9, 11, 12, 13, 14, 15, 16, 17, 18, and 19 postimmunization. </t>
+    <t>Except for the seven naive animals from the baseline group, nine animals (seven from the EAE and two from the control group) were sacrificed (at the same time of the day) at each of 13 time points after immunization, which are detailed as days 3, 5, 7, 9, 11, 12, 13, 14, 15, 16, 17, 18, and 19 postimmunization.</t>
   </si>
   <si>
     <t>0,10,20,30,40,50,60,90,120,150,180,210,240</t>
   </si>
   <si>
-    <t>13 Time Points (0, 10, 20, 30, 40, 50, 60, 90, 120, 150, 180, 210, 240 Minutes) 2 Biological Replicates. </t>
+    <t>13 Time Points (0, 10, 20, 30, 40, 50, 60, 90, 120, 150, 180, 210, 240 Minutes) 2 Biological Replicates.</t>
   </si>
   <si>
     <t>1,2,4,6,8,10,12,16,24,36,48,72,96</t>
   </si>
   <si>
-    <t>Total RNA was isolated from the cells at 1, 2, 4, 6, 8, 10, 12, 16, 24, 36, 48, 72, and 96 hours post-infection (h p.i.), respectively. </t>
+    <t>Total RNA was isolated from the cells at 1, 2, 4, 6, 8, 10, 12, 16, 24, 36, 48, 72, and 96 hours post-infection (h p.i.), respectively.</t>
   </si>
   <si>
     <t>10,13,14,16,18,20,22,24,27,29,32,34,37</t>
   </si>
   <si>
-    <t>The time-course study involved analysis of 13 samples (10h, 13h, 14h, 16h, 18h, 20h, 22h, 24h, 27h, 29h, 32h, 34h, 37h). </t>
+    <t>The time-course study involved analysis of 13 samples (10h, 13h, 14h, 16h, 18h, 20h, 22h, 24h, 27h, 29h, 32h, 34h, 37h).</t>
   </si>
   <si>
     <t>10,20,180,240,300,360,420,480,540,600,680,760</t>
@@ -711,7 +712,7 @@
     <t>0,1,1.5,2,3,6,9,12,24,48,96,144</t>
   </si>
   <si>
-    <t> Cells grown in separate plates were harvested at 12 different timepoints: t_0h, t_1h, t_1.5h, t_2h, t_3h, t_6h, t_9h, t_12h, t_24h, t_48h, t_96h, t_144h. </t>
+    <t>Cells grown in separate plates were harvested at 12 different timepoints: t_0h, t_1h, t_1.5h, t_2h, t_3h, t_6h, t_9h, t_12h, t_24h, t_48h, t_96h, t_144h.</t>
   </si>
   <si>
     <t>1,1.5,2,5,10,12,15,20,24,30,45,120</t>
@@ -765,7 +766,7 @@
     <t>24,28,32,36,40,44,48,52,56,60,64,68</t>
   </si>
   <si>
-    <t> Time points at CT24, 28, 32, 36, 40, 44, 48, 52, 56, 60, 64, and 68. </t>
+    <t>Time points at CT24, 28, 32, 36, 40, 44, 48, 52, 56, 60, 64, and 68.</t>
   </si>
   <si>
     <t>0,0.5,1,2,4,6,10,12,24,100,338,537</t>
@@ -870,13 +871,13 @@
     <t>11,19,22,24,26,28,31,32,35,37,38,41</t>
   </si>
   <si>
-    <t>Time-course study involved analysis of 12 samples (11h, 19h, 22h, 24h, 26h, 28h, 31h, 32h, 35h, 37h, 38h and 41h). </t>
+    <t>Time-course study involved analysis of 12 samples (11h, 19h, 22h, 24h, 26h, 28h, 31h, 32h, 35h, 37h, 38h and 41h).</t>
   </si>
   <si>
     <t>1,3,5,7,9,11,13,15,17,19,21,23</t>
   </si>
   <si>
-    <t>Samples were recovered at days 1, 3, 5, 7 (5%DSS), 9, 11, 13, 15 (2%DSS), 17, 19, 21 and 23 (0%DSS). </t>
+    <t>Samples were recovered at days 1, 3, 5, 7 (5%DSS), 9, 11, 13, 15 (2%DSS), 17, 19, 21 and 23 (0%DSS).</t>
   </si>
   <si>
     <t>0,1,2,3,4,5,24,48,72,96,120</t>
@@ -948,7 +949,7 @@
     <t>0,3,7,12,24,30,36,48,54,60,72</t>
   </si>
   <si>
-    <t> Cells samples were collected at 0, 3, 7, 12, 24, 30, 36, 48, 54, 60 or 72h post infection. </t>
+    <t>Cells samples were collected at 0, 3, 7, 12, 24, 30, 36, 48, 54, 60 or 72h post infection.</t>
   </si>
   <si>
     <t>1,2,3,12,18,24,30,36,42,48,305</t>
@@ -1023,7 +1024,7 @@
     <t>0,1,3,4,5,6,7,8,9,10,11</t>
   </si>
   <si>
-    <t> C57 and AJ strains examined at 0, 1, 3, 4, 5 ,6, 7, 8, 9, 10 and 11 weeks.;	</t>
+    <t>C57 and AJ strains examined at 0, 1, 3, 4, 5 ,6, 7, 8, 9, 10 and 11 weeks.;</t>
   </si>
   <si>
     <t>0,3,4,7,10,14,17,21,24,28,84</t>
@@ -1083,43 +1084,43 @@
     <t>0,0.25,0.5,1,1.5,2,4,6,8,12,18</t>
   </si>
   <si>
-    <t>Cells were washed, supplemented with warm media and harvested at 11 timepoints (0, .25, .5, 1, 1.5, 2, 4, 6, 8, 12, and 18 hours post-treatment). </t>
+    <t>Cells were washed, supplemented with warm media and harvested at 11 timepoints (0, .25, .5, 1, 1.5, 2, 4, 6, 8, 12, and 18 hours post-treatment).</t>
   </si>
   <si>
     <t>4,12,1,2,4,6,8,12,16,24,32</t>
   </si>
   <si>
-    <t> Daily mechanical loading was applied to the forearm (24 hours between loading sessions), and ulnae were sampled at indicated time points (4h, 12h, 1d, 2d, 4d, 6d, 8d, 12d, 16d, 24d, or 32d).</t>
+    <t>Daily mechanical loading was applied to the forearm (24 hours between loading sessions), and ulnae were sampled at indicated time points (4h, 12h, 1d, 2d, 4d, 6d, 8d, 12d, 16d, 24d, or 32d).</t>
   </si>
   <si>
     <t>0,6,12,18,24,36,48,4,7,9,14</t>
   </si>
   <si>
-    <t>Time course 0 hours, 6 hours, 12 hours, 18 hours, 24 hours, 36 hours, 48 hours, 4 days, 7 days, 9 days, and 14 days.;	</t>
-  </si>
-  <si>
-    <t>The time course includes 0 hr, 6 hr, 12 hr, 18 hr, 24 hr, 36 hr, 48 hr, 4 days, 7 days, 9 days and 14 days.;	</t>
+    <t>Time course 0 hours, 6 hours, 12 hours, 18 hours, 24 hours, 36 hours, 48 hours, 4 days, 7 days, 9 days, and 14 days.;</t>
+  </si>
+  <si>
+    <t>The time course includes 0 hr, 6 hr, 12 hr, 18 hr, 24 hr, 36 hr, 48 hr, 4 days, 7 days, 9 days and 14 days.;</t>
   </si>
   <si>
     <t>0,1,2,4,8,12,13,14,16,20,24</t>
   </si>
   <si>
-    <t>The experiment has involved sampling leaves at eleven different time points as follows: 0, 1, 2, 4, 8, 12, 13, 14, 16, 20, and 24 h (where time 0 is the onset of dark and 12 h is the onset of light). </t>
+    <t>The experiment has involved sampling leaves at eleven different time points as follows: 0, 1, 2, 4, 8, 12, 13, 14, 16, 20, and 24 h (where time 0 is the onset of dark and 12 h is the onset of light).</t>
   </si>
   <si>
     <t>1,5,6,7,8,10,12,17,18,19,22</t>
   </si>
   <si>
-    <t> These ranged in size from ~200 kb to 44 Mb, affecting chromosomes 1, 5, 6, 7, 8, 10, 12, 17, 18, 19, and 22. </t>
-  </si>
-  <si>
-    <t>Cells were collected after 180, 240, 300, 360, 420, 480, 540, 600, 680, and 760 min, and then crude RNA was extracted. </t>
+    <t>These ranged in size from ~200 kb to 44 Mb, affecting chromosomes 1, 5, 6, 7, 8, 10, 12, 17, 18, 19, and 22.</t>
+  </si>
+  <si>
+    <t>Cells were collected after 180, 240, 300, 360, 420, 480, 540, 600, 680, and 760 min, and then crude RNA was extracted.</t>
   </si>
   <si>
     <t>0,6,12,18,24,36,48,3,4,7</t>
   </si>
   <si>
-    <t>Time course: 0 hr, 6 hr, 12 hr, 18 hr, 24 hr, 36 hr, 48 hr, 3 days, 4 days, 7 days.;	</t>
+    <t>Time course: 0 hr, 6 hr, 12 hr, 18 hr, 24 hr, 36 hr, 48 hr, 3 days, 4 days, 7 days.;</t>
   </si>
   <si>
     <t>0,0.5,1,1.5,2,4,9,12,24,48</t>
@@ -1149,7 +1150,7 @@
     <t>0.5,3,6,8,12,18,24,48,72,96</t>
   </si>
   <si>
-    <t> Cells were harvested by centrifugation at 1000 rpm for 10 minutes, at the following times after induction, 0.5, 3, 6, 8, 12, 18, 24, 48, 72, and 96 hour(s). </t>
+    <t>Cells were harvested by centrifugation at 1000 rpm for 10 minutes, at the following times after induction, 0.5, 3, 6, 8, 12, 18, 24, 48, 72, and 96 hour(s).</t>
   </si>
   <si>
     <t>4,5,6,10,12,15,19,24,25,48</t>
@@ -1236,7 +1237,7 @@
     <t>0,10,20,30,40,50,60,90,120,150</t>
   </si>
   <si>
-    <t>10 Time Points (0,10,20,30,40,50,60,90,120,150 Minutes) 2 Biological Replicates. </t>
+    <t>10 Time Points (0,10,20,30,40,50,60,90,120,150 Minutes) 2 Biological Replicates.</t>
   </si>
   <si>
     <t>0,1,2,3,6,7,12,13,14,28</t>
@@ -1275,7 +1276,7 @@
     <t>0,7,12,24,30,36,48,54,60,72</t>
   </si>
   <si>
-    <t> Cells samples were collected at 0, 7, 12, 24, 30, 36, 48, 54, 60 or 72h post infection. </t>
+    <t>Cells samples were collected at 0, 7, 12, 24, 30, 36, 48, 54, 60 or 72h post infection.</t>
   </si>
   <si>
     <t>0,2,5,17,25,100,170,250,370,500</t>
@@ -1407,7 +1408,7 @@
     <t>12,16,20,32,36,40,52,56,60,72</t>
   </si>
   <si>
-    <t>Samples were withdrawn at different time points: after 12h, 16h, 20h, 32h, 36h, 40h, 52h, 56h, 60h and 72h from the initial inoculum. </t>
+    <t>Samples were withdrawn at different time points: after 12h, 16h, 20h, 32h, 36h, 40h, 52h, 56h, 60h and 72h from the initial inoculum.</t>
   </si>
   <si>
     <t>0,8,12,14,16,18,20,22,24,26</t>
@@ -1416,34 +1417,34 @@
     <t>0,1,12,24,2,4,6,9,12,15</t>
   </si>
   <si>
-    <t>Total RNA obteind from 10  different time points (0h, 1h, 12h, 24h, 2d, 4d, 6d, 9d, 12d, 15d) during adipogenesis from human Mesenchymal stem cell (MSC) to Adipocyte (ADP). </t>
+    <t>Total RNA obteind from 10  different time points (0h, 1h, 12h, 24h, 2d, 4d, 6d, 9d, 12d, 15d) during adipogenesis from human Mesenchymal stem cell (MSC) to Adipocyte (ADP).</t>
   </si>
   <si>
     <t>3,5,7,8,10,12,14,16,18,19</t>
   </si>
   <si>
-    <t>CL were collected between days 3-5 (early stage), 7-8 (mid), 10-12 (mid-late), 14-16 (late), or 18-19 (very-late) after the midcycle LH surge. </t>
+    <t>CL were collected between days 3-5 (early stage), 7-8 (mid), 10-12 (mid-late), 14-16 (late), or 18-19 (very-late) after the midcycle LH surge.</t>
   </si>
   <si>
     <t>15,30,45,1,2,3,4,5,6,7</t>
   </si>
   <si>
-    <t> Roots were excised from ten plants per treatment at ten time points (15�, 30�, 45� 1h, 2h, 3h, 4h, 5h, 6h, 7h) and frozen in liquid nitrogen. </t>
+    <t>Roots were excised from ten plants per treatment at ten time points (15�, 30�, 45� 1h, 2h, 3h, 4h, 5h, 6h, 7h) and frozen in liquid nitrogen.</t>
   </si>
   <si>
     <t>0.04,0.08,0.13,0.19,0.25,0.38,0.5,1,2,3</t>
   </si>
   <si>
-    <t> After three generations, the sparge gas was switched from air to O2-free N2 and samples were harvested after 0.04, 0.08, 0.13, 0.19, 0.25, 0.38, 0.5, 1, 2, and 3 generations of anaerobic growth in the presence of Antimycin A. </t>
-  </si>
-  <si>
-    <t>Time course : 0 hr, 6 hr, 12 hr, 18 hr, 24 hr, 36 hr, 48 hr, 3 days, 4 days, 7 days;	</t>
+    <t>After three generations, the sparge gas was switched from air to O2-free N2 and samples were harvested after 0.04, 0.08, 0.13, 0.19, 0.25, 0.38, 0.5, 1, 2, and 3 generations of anaerobic growth in the presence of Antimycin A.</t>
+  </si>
+  <si>
+    <t>Time course : 0 hr, 6 hr, 12 hr, 18 hr, 24 hr, 36 hr, 48 hr, 3 days, 4 days, 7 days;</t>
   </si>
   <si>
     <t>5,10,20,30,45,60,90,120,180,300</t>
   </si>
   <si>
-    <t>right away, after 5 mins, 10, 20, 30, 45, 60, 90, 120, 180, and 300 mins. </t>
+    <t>right away, after 5 mins, 10, 20, 30, 45, 60, 90, 120, 180, and 300 mins.</t>
   </si>
   <si>
     <t>0.5,1,2,4,6,8,10,12,16,24</t>
@@ -1452,19 +1453,16 @@
     <t>After adding human rIL-2 (100 U/mL, Chiron, IL-2 stimulation), cells were collected at time point 0.5, 1, 2, 4, 6, 8, 10, 12, 16 and 24 hours, at least 3 biological replicates were carried out for each time point.Total RNA were extracted from the cells and was hybridized on Affymetrix GeneChip Mouse Genome 430 2.0 Array.</t>
   </si>
   <si>
-    <t> Cells were collected after 180, 240, 300, 360, 420, 480, 540, 600, 680, and 760 min, and then crude RNA was extracted. </t>
-  </si>
-  <si>
     <t>2,3,4,5,6,7,8,9,10,11</t>
   </si>
   <si>
-    <t>In addition we have analyzed different passages of donor 1 (P2, P3, P4, P5, P6, P7, P8, P9, P10, and P11) to determine changes in the course of cellular aging.;	</t>
+    <t>In addition we have analyzed different passages of donor 1 (P2, P3, P4, P5, P6, P7, P8, P9, P10, and P11) to determine changes in the course of cellular aging.;</t>
   </si>
   <si>
     <t>12,24,36,2,3,4,5,6,7</t>
   </si>
   <si>
-    <t>Rats were then randomly allocated into timepoint groups to be sacrificed at either 12, 24, 36, day 2, 3, 4, 5, 6, 7. </t>
+    <t>Rats were then randomly allocated into timepoint groups to be sacrificed at either 12, 24, 36, day 2, 3, 4, 5, 6, 7.</t>
   </si>
   <si>
     <t>0,1,2,4,5,6,7,14,21</t>
@@ -1503,13 +1501,13 @@
     <t>0.08,0.25,0.5,1,2,4,8,16,24</t>
   </si>
   <si>
-    <t>The study investigated differential gene expression in Caco-2 cell line mRNA at 9 timepoints (t=0.08, 0.25, 0.5, 1, 2, 4, 8, 16, or 24h)  within 24 hours of exposure to H2O2 or manadione . </t>
+    <t>The study investigated differential gene expression in Caco-2 cell line mRNA at 9 timepoints (t=0.08, 0.25, 0.5, 1, 2, 4, 8, 16, or 24h)  within 24 hours of exposure to H2O2 or manadione .</t>
   </si>
   <si>
     <t>1,2,4,6,12,24,48,72,96</t>
   </si>
   <si>
-    <t>Total cell lysates were harvested in TRIzol reagent at 1, 2, 4, 6, 12, 24, 48, 72, 96 hours, including an undifferentiated control. </t>
+    <t>Total cell lysates were harvested in TRIzol reagent at 1, 2, 4, 6, 12, 24, 48, 72, 96 hours, including an undifferentiated control.</t>
   </si>
   <si>
     <t>27,51,75,99,123,147,171,195,219</t>
@@ -1572,13 +1570,13 @@
     <t>10,13,16,19,22,25,31,35,37</t>
   </si>
   <si>
-    <t>The time-course study involved analysis of 9 samples (10h, 13h, 16h, 19h, 22h, 25h, 31h, 35h, 37h). </t>
+    <t>The time-course study involved analysis of 9 samples (10h, 13h, 16h, 19h, 22h, 25h, 31h, 35h, 37h).</t>
   </si>
   <si>
     <t>0,1,3,5,7,10,14,28,56</t>
   </si>
   <si>
-    <t>In an Institutional Animal Care and Use Committee (IACUC) approved study, 27 adult male rats (Sprague Dawley, 400-425 g) were divided into nine groups: intact control (0 day), and 1, 3, 5, 7, 10, 14, 28, and 56 days post marrow ablation. </t>
+    <t>In an Institutional Animal Care and Use Committee (IACUC) approved study, 27 adult male rats (Sprague Dawley, 400-425 g) were divided into nine groups: intact control (0 day), and 1, 3, 5, 7, 10, 14, 28, and 56 days post marrow ablation.</t>
   </si>
   <si>
     <t>0.7,3,13,14,15,16,17,18,19</t>
@@ -1587,13 +1585,13 @@
     <t>14,15,16,17,18,19,20,21,40</t>
   </si>
   <si>
-    <t>The time-course study involved analysis of 9 samples (14hr, 15hr, 16hr, 17hr, 18hr, 19hr, 20hr, 21hr, 40hr). </t>
+    <t>The time-course study involved analysis of 9 samples (14hr, 15hr, 16hr, 17hr, 18hr, 19hr, 20hr, 21hr, 40hr).</t>
   </si>
   <si>
     <t>0,1,2,4,6,8,12,16,24</t>
   </si>
   <si>
-    <t> Doxycycline-induced and uninduced and Flp-In TREx 293/Vpr cells were collected 0, 1, 2, 4, 6, 8, 12, 16 and 24 hours post induction (hpi). </t>
+    <t>Doxycycline-induced and uninduced and Flp-In TREx 293/Vpr cells were collected 0, 1, 2, 4, 6, 8, 12, 16 and 24 hours post induction (hpi).</t>
   </si>
   <si>
     <t>1,3,6,9,10,13,14,18,20</t>
@@ -1665,7 +1663,7 @@
     <t>0.5,1,2,4,6,8,12,16,18</t>
   </si>
   <si>
-    <t>albicans cells and these infected fish were collected at 0.5, 1, 2, 4, 6, 8, 12, 16, 18 hpi. </t>
+    <t>albicans cells and these infected fish were collected at 0.5, 1, 2, 4, 6, 8, 12, 16, 18 hpi.</t>
   </si>
   <si>
     <t>13,14,15,16,53,63,69,72,76</t>
@@ -1704,19 +1702,19 @@
     <t>0,3,7,12,18,24,30,36,48</t>
   </si>
   <si>
-    <t>Calu-3 cells were infected with A/CA/04/2009 Influenza virus at MOI of 3, samples were collected 0,3,7,12,18, 24, 30, 36 and 48 hpi. </t>
+    <t>Calu-3 cells were infected with A/CA/04/2009 Influenza virus at MOI of 3, samples were collected 0,3,7,12,18, 24, 30, 36 and 48 hpi.</t>
   </si>
   <si>
     <t>2,3,4,5,6,7,8,9,10</t>
   </si>
   <si>
-    <t>At different stages of the sporulation process (2, 3, 4, 5, 6, 7, 8, 9 and 10 hours) RNA was extracted for microarray hybridizations. </t>
+    <t>At different stages of the sporulation process (2, 3, 4, 5, 6, 7, 8, 9 and 10 hours) RNA was extracted for microarray hybridizations.</t>
   </si>
   <si>
     <t>0.02,4,10,21,22,227,450,562,971</t>
   </si>
   <si>
-    <t>For the A/Netherlands/602/09-infected and mock-infected cells, samples were collected at 0, 3, 7, 12, 18, 24, 30, 36, and 48 hours post-infection (h.p.i.). </t>
+    <t>For the A/Netherlands/602/09-infected and mock-infected cells, samples were collected at 0, 3, 7, 12, 18, 24, 30, 36, and 48 hours post-infection (h.p.i.).</t>
   </si>
   <si>
     <t>1,3,7,12,16,20,25,31,38</t>
@@ -1770,7 +1768,7 @@
     <t>2,4,6,8,10,12,14,16,18</t>
   </si>
   <si>
-    <t> Cells expressing CFP were returned to culture, subjected to an osteoblast differentiation cocktail and RNA was collected at 2, 4, 6, 8, 10, 12, 14, 16 and 18 days post differentiation.;	</t>
+    <t>Cells expressing CFP were returned to culture, subjected to an osteoblast differentiation cocktail and RNA was collected at 2, 4, 6, 8, 10, 12, 14, 16 and 18 days post differentiation.;</t>
   </si>
   <si>
     <t>0,1,2,3,5,6,12,24,48</t>
@@ -1824,7 +1822,7 @@
     <t>1,2,4,6,8,12,16,20,24</t>
   </si>
   <si>
-    <t>Total RNA was extracted from cells at 1, 2, 4, 6, 8, 12, 16, 20 and 24 hours after irradiation. </t>
+    <t>Total RNA was extracted from cells at 1, 2, 4, 6, 8, 12, 16, 20 and 24 hours after irradiation.</t>
   </si>
   <si>
     <t>0,1,2,3,24,30,60,90,120</t>
@@ -1842,7 +1840,7 @@
     <t>12,24,2,3,4,6,7,8,9</t>
   </si>
   <si>
-    <t> Cells were harvested at 12 hrs, 24hrs, 2 days, 3 days, 4days, 6 days, 7 days, 8 days, and 9 days of growth in culture using Matrisperse (Falcon, Becton-Dickinson Labware, Franklin Lakes, NJ) and RNA collected. </t>
+    <t>Cells were harvested at 12 hrs, 24hrs, 2 days, 3 days, 4days, 6 days, 7 days, 8 days, and 9 days of growth in culture using Matrisperse (Falcon, Becton-Dickinson Labware, Franklin Lakes, NJ) and RNA collected.</t>
   </si>
   <si>
     <t>1,2,3,4,5,6,7,8,12</t>
@@ -1854,52 +1852,52 @@
     <t>5,15,30,60,120,180,240,300,360</t>
   </si>
   <si>
-    <t> Samples were taken immediately prior to transition to acetate (reference sample) and at 5, 15, 30, 60, 120, 180, 240, 300, and 360 minutes after transition.</t>
+    <t>Samples were taken immediately prior to transition to acetate (reference sample) and at 5, 15, 30, 60, 120, 180, 240, 300, and 360 minutes after transition.</t>
   </si>
   <si>
     <t>0,3,6,12,24,48,72,120,168</t>
   </si>
   <si>
-    <t>In this study presented here, Middle Cerebral Artery Occlusion stroke model was established by using embolus and the brain samples of stroke model were harvested at 0hrs, 3hrs, 6hrs, 12hrs, 24hrs, 48hrs, 72hrs, 120hrs and 168hrs. </t>
+    <t>In this study presented here, Middle Cerebral Artery Occlusion stroke model was established by using embolus and the brain samples of stroke model were harvested at 0hrs, 3hrs, 6hrs, 12hrs, 24hrs, 48hrs, 72hrs, 120hrs and 168hrs.</t>
   </si>
   <si>
     <t>0,7,12,24,36,36,48,60,72</t>
   </si>
   <si>
-    <t> Cells samples were collected at 0, 7, 12, 24, 36, 36, 48, 60 or 72h post infection. </t>
+    <t>Cells samples were collected at 0, 7, 12, 24, 36, 36, 48, 60 or 72h post infection.</t>
   </si>
   <si>
     <t>30,1,2,4,8,12,24,48,72</t>
   </si>
   <si>
-    <t>mRNA was isolated at 30 minutes, 1, 2, 4, 8, 12, 24, 48, and 72 hours after seeding.;	</t>
-  </si>
-  <si>
-    <t>In this study presented here, Middle Cerebral Artery Occlusion stroke model was established by using embolus and the brain samples of stroke model were harvestd at 0hrs, 3hrs, 6hrs, 12hrs, 24hrs, 48hrs, 72hrs, 120hrs and 168hrs. </t>
+    <t>mRNA was isolated at 30 minutes, 1, 2, 4, 8, 12, 24, 48, and 72 hours after seeding.;</t>
+  </si>
+  <si>
+    <t>In this study presented here, Middle Cerebral Artery Occlusion stroke model was established by using embolus and the brain samples of stroke model were harvestd at 0hrs, 3hrs, 6hrs, 12hrs, 24hrs, 48hrs, 72hrs, 120hrs and 168hrs.</t>
   </si>
   <si>
     <t>0,6,12,18,24,48,72,96,120</t>
   </si>
   <si>
-    <t>orontii infection were assayed in wild-type Col-0 plants at 6, 12, 18, 24, 48, 72, 96, and 120 hours after inoculation of adult leaves. </t>
+    <t>orontii infection were assayed in wild-type Col-0 plants at 6, 12, 18, 24, 48, 72, 96, and 120 hours after inoculation of adult leaves.</t>
   </si>
   <si>
     <t>66,78,90,108,120,144,12,24,48</t>
   </si>
   <si>
-    <t>Each microarray slide contained a different combination of 2 of the 9 developmental stages used in the experiment (66 hpf, 78 hpf, 90 hpf, 108 hpf, 120 hpf, 144 hpf, 12 hpi, 24 hpi, 48 hpi). </t>
+    <t>Each microarray slide contained a different combination of 2 of the 9 developmental stages used in the experiment (66 hpf, 78 hpf, 90 hpf, 108 hpf, 120 hpf, 144 hpf, 12 hpi, 24 hpi, 48 hpi).</t>
   </si>
   <si>
     <t>0,2,7,12,17,22,27,32,37</t>
   </si>
   <si>
-    <t>Gene expression was measured at nine time intervals (0, 2, 7, 12, 17, 22, 27, 32, 37 minutes) during phage infection.;	</t>
+    <t>Gene expression was measured at nine time intervals (0, 2, 7, 12, 17, 22, 27, 32, 37 minutes) during phage infection.;</t>
   </si>
   <si>
     <t>0.5,1,2,4,6,12,24,48,72</t>
   </si>
   <si>
-    <t>Total RNA obtained from activated and IL-4 &amp; anti-IL-12 treated cord blood CD4+ T cells, 0.5, 1, 2, 4, 6, 12, 24, 48, and 72 hours after initiation of the cultures, compared to cells which were only activated. </t>
+    <t>Total RNA obtained from activated and IL-4 &amp; anti-IL-12 treated cord blood CD4+ T cells, 0.5, 1, 2, 4, 6, 12, 24, 48, and 72 hours after initiation of the cultures, compared to cells which were only activated.</t>
   </si>
   <si>
     <t>-18,-4,0,2,4,6,8,10,12</t>
@@ -1911,13 +1909,13 @@
     <t>1,2.5,4,6,8,10,12,14,20</t>
   </si>
   <si>
-    <t>Temporal expression profiling of hindlimb muscle of beta- and gamma-sarcoglycan deficient mice aged 1, 2.5, 4, 6, 8, 10, 12, 14 and 20 weeks.;	</t>
+    <t>Temporal expression profiling of hindlimb muscle of beta- and gamma-sarcoglycan deficient mice aged 1, 2.5, 4, 6, 8, 10, 12, 14 and 20 weeks.;</t>
   </si>
   <si>
     <t>1,3,5,7,10,14,21,28,35</t>
   </si>
   <si>
-    <t>METHODS: C57BL/6 mice were sacrificed and kidneys were harvested at embryonic day E19.5, and postnatal days P1, P3, P5, P7, P10, P14, P21, P28 and P35. </t>
+    <t>METHODS: C57BL/6 mice were sacrificed and kidneys were harvested at embryonic day E19.5, and postnatal days P1, P3, P5, P7, P10, P14, P21, P28 and P35.</t>
   </si>
   <si>
     <t>0,2,4,6,8,12,16,20,24</t>
@@ -1929,7 +1927,7 @@
     <t>2,3,4,5,6,7,8,10,11</t>
   </si>
   <si>
-    <t>In addition we have analyzed different passages of donor 1 (P2, P3, P4, P5, P6, P7, P8, P10, and P11) to determine changes in the course of cellular aging. </t>
+    <t>In addition we have analyzed different passages of donor 1 (P2, P3, P4, P5, P6, P7, P8, P10, and P11) to determine changes in the course of cellular aging.</t>
   </si>
 </sst>
 </file>
@@ -1968,6 +1966,7 @@
       <color rgb="FF000000"/>
       <name val="WenQuanYi Zen Hei Sharp"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2041,7 +2040,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8485,7 +8484,7 @@
         <v>14</v>
       </c>
       <c r="D565" s="0" t="s">
-        <v>471</v>
+        <v>358</v>
       </c>
     </row>
     <row r="566" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8493,13 +8492,13 @@
         <v>10</v>
       </c>
       <c r="B566" s="0" t="s">
+        <v>471</v>
+      </c>
+      <c r="C566" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D566" s="0" t="s">
         <v>472</v>
-      </c>
-      <c r="C566" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D566" s="0" t="s">
-        <v>473</v>
       </c>
     </row>
     <row r="567" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8507,13 +8506,13 @@
         <v>9</v>
       </c>
       <c r="B567" s="0" t="s">
+        <v>473</v>
+      </c>
+      <c r="C567" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D567" s="0" t="s">
         <v>474</v>
-      </c>
-      <c r="C567" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D567" s="0" t="s">
-        <v>475</v>
       </c>
     </row>
     <row r="568" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8521,7 +8520,7 @@
         <v>9</v>
       </c>
       <c r="B568" s="0" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C568" s="0" t="s">
         <v>2</v>
@@ -8532,7 +8531,7 @@
         <v>9</v>
       </c>
       <c r="B569" s="0" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C569" s="0" t="s">
         <v>2</v>
@@ -8543,7 +8542,7 @@
         <v>9</v>
       </c>
       <c r="B570" s="0" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C570" s="0" t="s">
         <v>2</v>
@@ -8554,7 +8553,7 @@
         <v>9</v>
       </c>
       <c r="B571" s="0" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C571" s="0" t="s">
         <v>2</v>
@@ -8565,7 +8564,7 @@
         <v>9</v>
       </c>
       <c r="B572" s="0" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C572" s="0" t="s">
         <v>2</v>
@@ -8576,7 +8575,7 @@
         <v>9</v>
       </c>
       <c r="B573" s="0" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C573" s="0" t="s">
         <v>2</v>
@@ -8587,7 +8586,7 @@
         <v>9</v>
       </c>
       <c r="B574" s="0" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C574" s="0" t="s">
         <v>2</v>
@@ -8598,7 +8597,7 @@
         <v>9</v>
       </c>
       <c r="B575" s="0" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C575" s="0" t="s">
         <v>2</v>
@@ -8609,7 +8608,7 @@
         <v>9</v>
       </c>
       <c r="B576" s="0" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C576" s="0" t="s">
         <v>2</v>
@@ -8620,7 +8619,7 @@
         <v>9</v>
       </c>
       <c r="B577" s="0" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C577" s="0" t="s">
         <v>2</v>
@@ -8631,7 +8630,7 @@
         <v>9</v>
       </c>
       <c r="B578" s="0" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C578" s="0" t="s">
         <v>2</v>
@@ -8642,7 +8641,7 @@
         <v>9</v>
       </c>
       <c r="B579" s="0" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C579" s="0" t="s">
         <v>2</v>
@@ -8653,7 +8652,7 @@
         <v>9</v>
       </c>
       <c r="B580" s="0" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C580" s="0" t="s">
         <v>2</v>
@@ -8664,7 +8663,7 @@
         <v>9</v>
       </c>
       <c r="B581" s="0" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C581" s="0" t="s">
         <v>2</v>
@@ -8675,13 +8674,13 @@
         <v>9</v>
       </c>
       <c r="B582" s="0" t="s">
+        <v>486</v>
+      </c>
+      <c r="C582" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D582" s="0" t="s">
         <v>487</v>
-      </c>
-      <c r="C582" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D582" s="0" t="s">
-        <v>488</v>
       </c>
     </row>
     <row r="583" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8689,13 +8688,13 @@
         <v>9</v>
       </c>
       <c r="B583" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="C583" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D583" s="0" t="s">
         <v>489</v>
-      </c>
-      <c r="C583" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D583" s="0" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="584" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8703,7 +8702,7 @@
         <v>9</v>
       </c>
       <c r="B584" s="0" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C584" s="0" t="s">
         <v>2</v>
@@ -8714,7 +8713,7 @@
         <v>9</v>
       </c>
       <c r="B585" s="0" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C585" s="0" t="s">
         <v>2</v>
@@ -8725,7 +8724,7 @@
         <v>9</v>
       </c>
       <c r="B586" s="0" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C586" s="0" t="s">
         <v>2</v>
@@ -8736,7 +8735,7 @@
         <v>9</v>
       </c>
       <c r="B587" s="0" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C587" s="0" t="s">
         <v>2</v>
@@ -8747,7 +8746,7 @@
         <v>9</v>
       </c>
       <c r="B588" s="0" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C588" s="0" t="s">
         <v>2</v>
@@ -8758,7 +8757,7 @@
         <v>9</v>
       </c>
       <c r="B589" s="0" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C589" s="0" t="s">
         <v>2</v>
@@ -8769,7 +8768,7 @@
         <v>9</v>
       </c>
       <c r="B590" s="0" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C590" s="0" t="s">
         <v>2</v>
@@ -8780,7 +8779,7 @@
         <v>9</v>
       </c>
       <c r="B591" s="0" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C591" s="0" t="s">
         <v>2</v>
@@ -8791,7 +8790,7 @@
         <v>9</v>
       </c>
       <c r="B592" s="0" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C592" s="0" t="s">
         <v>2</v>
@@ -8802,7 +8801,7 @@
         <v>9</v>
       </c>
       <c r="B593" s="0" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C593" s="0" t="s">
         <v>2</v>
@@ -8813,7 +8812,7 @@
         <v>9</v>
       </c>
       <c r="B594" s="0" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C594" s="0" t="s">
         <v>2</v>
@@ -8824,7 +8823,7 @@
         <v>9</v>
       </c>
       <c r="B595" s="0" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C595" s="0" t="s">
         <v>2</v>
@@ -8835,7 +8834,7 @@
         <v>9</v>
       </c>
       <c r="B596" s="0" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C596" s="0" t="s">
         <v>2</v>
@@ -8846,7 +8845,7 @@
         <v>9</v>
       </c>
       <c r="B597" s="0" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C597" s="0" t="s">
         <v>2</v>
@@ -8857,7 +8856,7 @@
         <v>9</v>
       </c>
       <c r="B598" s="0" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C598" s="0" t="s">
         <v>2</v>
@@ -8868,7 +8867,7 @@
         <v>9</v>
       </c>
       <c r="B599" s="0" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C599" s="0" t="s">
         <v>2</v>
@@ -8879,7 +8878,7 @@
         <v>9</v>
       </c>
       <c r="B600" s="0" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C600" s="0" t="s">
         <v>2</v>
@@ -8890,7 +8889,7 @@
         <v>9</v>
       </c>
       <c r="B601" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C601" s="0" t="s">
         <v>2</v>
@@ -8901,7 +8900,7 @@
         <v>9</v>
       </c>
       <c r="B602" s="0" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C602" s="0" t="s">
         <v>2</v>
@@ -8912,7 +8911,7 @@
         <v>9</v>
       </c>
       <c r="B603" s="0" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C603" s="0" t="s">
         <v>2</v>
@@ -8923,7 +8922,7 @@
         <v>9</v>
       </c>
       <c r="B604" s="0" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C604" s="0" t="s">
         <v>2</v>
@@ -8934,7 +8933,7 @@
         <v>9</v>
       </c>
       <c r="B605" s="0" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C605" s="0" t="s">
         <v>2</v>
@@ -8945,7 +8944,7 @@
         <v>9</v>
       </c>
       <c r="B606" s="0" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C606" s="0" t="s">
         <v>2</v>
@@ -8956,7 +8955,7 @@
         <v>9</v>
       </c>
       <c r="B607" s="0" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C607" s="0" t="s">
         <v>2</v>
@@ -8967,7 +8966,7 @@
         <v>9</v>
       </c>
       <c r="B608" s="0" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C608" s="0" t="s">
         <v>2</v>
@@ -8978,13 +8977,13 @@
         <v>9</v>
       </c>
       <c r="B609" s="0" t="s">
+        <v>509</v>
+      </c>
+      <c r="C609" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D609" s="0" t="s">
         <v>510</v>
-      </c>
-      <c r="C609" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D609" s="0" t="s">
-        <v>511</v>
       </c>
     </row>
     <row r="610" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8992,13 +8991,13 @@
         <v>9</v>
       </c>
       <c r="B610" s="0" t="s">
+        <v>511</v>
+      </c>
+      <c r="C610" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D610" s="0" t="s">
         <v>512</v>
-      </c>
-      <c r="C610" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D610" s="0" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="611" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9006,7 +9005,7 @@
         <v>9</v>
       </c>
       <c r="B611" s="0" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C611" s="0" t="s">
         <v>2</v>
@@ -9017,13 +9016,13 @@
         <v>9</v>
       </c>
       <c r="B612" s="0" t="s">
+        <v>514</v>
+      </c>
+      <c r="C612" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D612" s="0" t="s">
         <v>515</v>
-      </c>
-      <c r="C612" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D612" s="0" t="s">
-        <v>516</v>
       </c>
     </row>
     <row r="613" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9031,13 +9030,13 @@
         <v>9</v>
       </c>
       <c r="B613" s="0" t="s">
+        <v>516</v>
+      </c>
+      <c r="C613" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D613" s="0" t="s">
         <v>517</v>
-      </c>
-      <c r="C613" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D613" s="0" t="s">
-        <v>518</v>
       </c>
     </row>
     <row r="614" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9045,7 +9044,7 @@
         <v>9</v>
       </c>
       <c r="B614" s="0" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C614" s="0" t="s">
         <v>2</v>
@@ -9056,7 +9055,7 @@
         <v>9</v>
       </c>
       <c r="B615" s="0" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C615" s="0" t="s">
         <v>2</v>
@@ -9067,7 +9066,7 @@
         <v>9</v>
       </c>
       <c r="B616" s="0" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C616" s="0" t="s">
         <v>2</v>
@@ -9078,7 +9077,7 @@
         <v>9</v>
       </c>
       <c r="B617" s="0" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C617" s="0" t="s">
         <v>2</v>
@@ -9089,7 +9088,7 @@
         <v>9</v>
       </c>
       <c r="B618" s="0" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C618" s="0" t="s">
         <v>2</v>
@@ -9100,7 +9099,7 @@
         <v>9</v>
       </c>
       <c r="B619" s="0" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C619" s="0" t="s">
         <v>2</v>
@@ -9111,7 +9110,7 @@
         <v>9</v>
       </c>
       <c r="B620" s="0" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C620" s="0" t="s">
         <v>2</v>
@@ -9122,7 +9121,7 @@
         <v>9</v>
       </c>
       <c r="B621" s="0" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C621" s="0" t="s">
         <v>2</v>
@@ -9133,7 +9132,7 @@
         <v>9</v>
       </c>
       <c r="B622" s="0" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C622" s="0" t="s">
         <v>2</v>
@@ -9144,7 +9143,7 @@
         <v>9</v>
       </c>
       <c r="B623" s="0" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C623" s="0" t="s">
         <v>2</v>
@@ -9155,7 +9154,7 @@
         <v>9</v>
       </c>
       <c r="B624" s="0" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C624" s="0" t="s">
         <v>2</v>
@@ -9166,7 +9165,7 @@
         <v>9</v>
       </c>
       <c r="B625" s="0" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C625" s="0" t="s">
         <v>2</v>
@@ -9177,7 +9176,7 @@
         <v>9</v>
       </c>
       <c r="B626" s="0" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C626" s="0" t="s">
         <v>2</v>
@@ -9188,7 +9187,7 @@
         <v>9</v>
       </c>
       <c r="B627" s="0" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C627" s="0" t="s">
         <v>2</v>
@@ -9199,7 +9198,7 @@
         <v>9</v>
       </c>
       <c r="B628" s="0" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C628" s="0" t="s">
         <v>2</v>
@@ -9210,7 +9209,7 @@
         <v>9</v>
       </c>
       <c r="B629" s="0" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C629" s="0" t="s">
         <v>2</v>
@@ -9221,7 +9220,7 @@
         <v>9</v>
       </c>
       <c r="B630" s="0" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C630" s="0" t="s">
         <v>2</v>
@@ -9232,7 +9231,7 @@
         <v>9</v>
       </c>
       <c r="B631" s="0" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C631" s="0" t="s">
         <v>2</v>
@@ -9243,7 +9242,7 @@
         <v>9</v>
       </c>
       <c r="B632" s="0" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C632" s="0" t="s">
         <v>2</v>
@@ -9254,7 +9253,7 @@
         <v>9</v>
       </c>
       <c r="B633" s="0" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C633" s="0" t="s">
         <v>2</v>
@@ -9265,7 +9264,7 @@
         <v>9</v>
       </c>
       <c r="B634" s="0" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C634" s="0" t="s">
         <v>2</v>
@@ -9276,7 +9275,7 @@
         <v>9</v>
       </c>
       <c r="B635" s="0" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C635" s="0" t="s">
         <v>2</v>
@@ -9287,7 +9286,7 @@
         <v>9</v>
       </c>
       <c r="B636" s="0" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C636" s="0" t="s">
         <v>2</v>
@@ -9298,7 +9297,7 @@
         <v>9</v>
       </c>
       <c r="B637" s="0" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C637" s="0" t="s">
         <v>2</v>
@@ -9309,13 +9308,13 @@
         <v>9</v>
       </c>
       <c r="B638" s="0" t="s">
+        <v>540</v>
+      </c>
+      <c r="C638" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D638" s="0" t="s">
         <v>541</v>
-      </c>
-      <c r="C638" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D638" s="0" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="639" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9323,13 +9322,13 @@
         <v>9</v>
       </c>
       <c r="B639" s="0" t="s">
+        <v>540</v>
+      </c>
+      <c r="C639" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D639" s="0" t="s">
         <v>541</v>
-      </c>
-      <c r="C639" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D639" s="0" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="640" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9337,7 +9336,7 @@
         <v>9</v>
       </c>
       <c r="B640" s="0" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C640" s="0" t="s">
         <v>2</v>
@@ -9348,7 +9347,7 @@
         <v>9</v>
       </c>
       <c r="B641" s="0" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C641" s="0" t="s">
         <v>2</v>
@@ -9359,7 +9358,7 @@
         <v>9</v>
       </c>
       <c r="B642" s="0" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C642" s="0" t="s">
         <v>2</v>
@@ -9370,7 +9369,7 @@
         <v>9</v>
       </c>
       <c r="B643" s="0" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C643" s="0" t="s">
         <v>2</v>
@@ -9381,7 +9380,7 @@
         <v>9</v>
       </c>
       <c r="B644" s="0" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C644" s="0" t="s">
         <v>2</v>
@@ -9392,7 +9391,7 @@
         <v>9</v>
       </c>
       <c r="B645" s="0" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C645" s="0" t="s">
         <v>2</v>
@@ -9403,7 +9402,7 @@
         <v>9</v>
       </c>
       <c r="B646" s="0" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C646" s="0" t="s">
         <v>2</v>
@@ -9414,7 +9413,7 @@
         <v>9</v>
       </c>
       <c r="B647" s="0" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C647" s="0" t="s">
         <v>2</v>
@@ -9425,7 +9424,7 @@
         <v>9</v>
       </c>
       <c r="B648" s="0" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C648" s="0" t="s">
         <v>2</v>
@@ -9436,7 +9435,7 @@
         <v>9</v>
       </c>
       <c r="B649" s="0" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C649" s="0" t="s">
         <v>2</v>
@@ -9447,7 +9446,7 @@
         <v>9</v>
       </c>
       <c r="B650" s="0" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C650" s="0" t="s">
         <v>2</v>
@@ -9458,7 +9457,7 @@
         <v>9</v>
       </c>
       <c r="B651" s="0" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C651" s="0" t="s">
         <v>2</v>
@@ -9469,7 +9468,7 @@
         <v>9</v>
       </c>
       <c r="B652" s="0" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C652" s="0" t="s">
         <v>2</v>
@@ -9480,13 +9479,13 @@
         <v>9</v>
       </c>
       <c r="B653" s="0" t="s">
+        <v>553</v>
+      </c>
+      <c r="C653" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D653" s="0" t="s">
         <v>554</v>
-      </c>
-      <c r="C653" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D653" s="0" t="s">
-        <v>555</v>
       </c>
     </row>
     <row r="654" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9494,13 +9493,13 @@
         <v>9</v>
       </c>
       <c r="B654" s="0" t="s">
+        <v>555</v>
+      </c>
+      <c r="C654" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D654" s="0" t="s">
         <v>556</v>
-      </c>
-      <c r="C654" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D654" s="0" t="s">
-        <v>557</v>
       </c>
     </row>
     <row r="655" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9508,13 +9507,13 @@
         <v>9</v>
       </c>
       <c r="B655" s="0" t="s">
+        <v>555</v>
+      </c>
+      <c r="C655" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D655" s="0" t="s">
         <v>556</v>
-      </c>
-      <c r="C655" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D655" s="0" t="s">
-        <v>557</v>
       </c>
     </row>
     <row r="656" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9522,7 +9521,7 @@
         <v>9</v>
       </c>
       <c r="B656" s="0" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C656" s="0" t="s">
         <v>2</v>
@@ -9533,7 +9532,7 @@
         <v>9</v>
       </c>
       <c r="B657" s="0" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C657" s="0" t="s">
         <v>2</v>
@@ -9544,13 +9543,13 @@
         <v>9</v>
       </c>
       <c r="B658" s="0" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C658" s="0" t="s">
         <v>14</v>
       </c>
       <c r="D658" s="0" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="659" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9558,7 +9557,7 @@
         <v>9</v>
       </c>
       <c r="B659" s="0" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C659" s="0" t="s">
         <v>2</v>
@@ -9569,7 +9568,7 @@
         <v>9</v>
       </c>
       <c r="B660" s="0" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C660" s="0" t="s">
         <v>2</v>
@@ -9580,7 +9579,7 @@
         <v>9</v>
       </c>
       <c r="B661" s="0" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C661" s="0" t="s">
         <v>2</v>
@@ -9591,7 +9590,7 @@
         <v>9</v>
       </c>
       <c r="B662" s="0" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C662" s="0" t="s">
         <v>2</v>
@@ -9613,13 +9612,13 @@
         <v>9</v>
       </c>
       <c r="B664" s="0" t="s">
+        <v>563</v>
+      </c>
+      <c r="C664" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D664" s="0" t="s">
         <v>564</v>
-      </c>
-      <c r="C664" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D664" s="0" t="s">
-        <v>565</v>
       </c>
     </row>
     <row r="665" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9627,7 +9626,7 @@
         <v>9</v>
       </c>
       <c r="B665" s="0" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C665" s="0" t="s">
         <v>2</v>
@@ -9638,7 +9637,7 @@
         <v>9</v>
       </c>
       <c r="B666" s="0" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C666" s="0" t="s">
         <v>2</v>
@@ -9649,7 +9648,7 @@
         <v>9</v>
       </c>
       <c r="B667" s="0" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C667" s="0" t="s">
         <v>2</v>
@@ -9660,7 +9659,7 @@
         <v>9</v>
       </c>
       <c r="B668" s="0" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C668" s="0" t="s">
         <v>2</v>
@@ -9671,7 +9670,7 @@
         <v>9</v>
       </c>
       <c r="B669" s="0" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C669" s="0" t="s">
         <v>2</v>
@@ -9682,7 +9681,7 @@
         <v>9</v>
       </c>
       <c r="B670" s="0" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C670" s="0" t="s">
         <v>2</v>
@@ -9693,7 +9692,7 @@
         <v>9</v>
       </c>
       <c r="B671" s="0" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="C671" s="0" t="s">
         <v>2</v>
@@ -9704,7 +9703,7 @@
         <v>9</v>
       </c>
       <c r="B672" s="0" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="C672" s="0" t="s">
         <v>2</v>
@@ -9715,7 +9714,7 @@
         <v>9</v>
       </c>
       <c r="B673" s="0" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C673" s="0" t="s">
         <v>2</v>
@@ -9726,7 +9725,7 @@
         <v>9</v>
       </c>
       <c r="B674" s="0" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C674" s="0" t="s">
         <v>2</v>
@@ -9737,7 +9736,7 @@
         <v>9</v>
       </c>
       <c r="B675" s="0" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C675" s="0" t="s">
         <v>2</v>
@@ -9748,13 +9747,13 @@
         <v>9</v>
       </c>
       <c r="B676" s="0" t="s">
+        <v>575</v>
+      </c>
+      <c r="C676" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D676" s="0" t="s">
         <v>576</v>
-      </c>
-      <c r="C676" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D676" s="0" t="s">
-        <v>577</v>
       </c>
     </row>
     <row r="677" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9762,7 +9761,7 @@
         <v>9</v>
       </c>
       <c r="B677" s="0" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C677" s="0" t="s">
         <v>2</v>
@@ -9773,7 +9772,7 @@
         <v>9</v>
       </c>
       <c r="B678" s="0" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C678" s="0" t="s">
         <v>2</v>
@@ -9784,7 +9783,7 @@
         <v>9</v>
       </c>
       <c r="B679" s="0" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C679" s="0" t="s">
         <v>2</v>
@@ -9795,7 +9794,7 @@
         <v>9</v>
       </c>
       <c r="B680" s="0" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C680" s="0" t="s">
         <v>2</v>
@@ -9806,7 +9805,7 @@
         <v>9</v>
       </c>
       <c r="B681" s="0" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C681" s="0" t="s">
         <v>2</v>
@@ -9817,7 +9816,7 @@
         <v>9</v>
       </c>
       <c r="B682" s="0" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C682" s="0" t="s">
         <v>2</v>
@@ -9828,7 +9827,7 @@
         <v>9</v>
       </c>
       <c r="B683" s="0" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C683" s="0" t="s">
         <v>2</v>
@@ -9839,7 +9838,7 @@
         <v>9</v>
       </c>
       <c r="B684" s="0" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C684" s="0" t="s">
         <v>2</v>
@@ -9850,7 +9849,7 @@
         <v>9</v>
       </c>
       <c r="B685" s="0" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C685" s="0" t="s">
         <v>2</v>
@@ -9861,7 +9860,7 @@
         <v>9</v>
       </c>
       <c r="B686" s="0" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C686" s="0" t="s">
         <v>2</v>
@@ -9872,7 +9871,7 @@
         <v>9</v>
       </c>
       <c r="B687" s="0" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C687" s="0" t="s">
         <v>2</v>
@@ -9883,7 +9882,7 @@
         <v>9</v>
       </c>
       <c r="B688" s="0" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C688" s="0" t="s">
         <v>2</v>
@@ -9894,7 +9893,7 @@
         <v>9</v>
       </c>
       <c r="B689" s="0" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C689" s="0" t="s">
         <v>2</v>
@@ -9905,7 +9904,7 @@
         <v>9</v>
       </c>
       <c r="B690" s="0" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C690" s="0" t="s">
         <v>2</v>
@@ -9916,7 +9915,7 @@
         <v>9</v>
       </c>
       <c r="B691" s="0" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="C691" s="0" t="s">
         <v>2</v>
@@ -9927,7 +9926,7 @@
         <v>9</v>
       </c>
       <c r="B692" s="0" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C692" s="0" t="s">
         <v>2</v>
@@ -9938,7 +9937,7 @@
         <v>9</v>
       </c>
       <c r="B693" s="0" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C693" s="0" t="s">
         <v>2</v>
@@ -9949,7 +9948,7 @@
         <v>9</v>
       </c>
       <c r="B694" s="0" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C694" s="0" t="s">
         <v>2</v>
@@ -9960,7 +9959,7 @@
         <v>9</v>
       </c>
       <c r="B695" s="0" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C695" s="0" t="s">
         <v>2</v>
@@ -9971,7 +9970,7 @@
         <v>9</v>
       </c>
       <c r="B696" s="0" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C696" s="0" t="s">
         <v>2</v>
@@ -9982,13 +9981,13 @@
         <v>9</v>
       </c>
       <c r="B697" s="0" t="s">
+        <v>593</v>
+      </c>
+      <c r="C697" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D697" s="0" t="s">
         <v>594</v>
-      </c>
-      <c r="C697" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D697" s="0" t="s">
-        <v>595</v>
       </c>
     </row>
     <row r="698" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9996,7 +9995,7 @@
         <v>9</v>
       </c>
       <c r="B698" s="0" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C698" s="0" t="s">
         <v>2</v>
@@ -10007,7 +10006,7 @@
         <v>9</v>
       </c>
       <c r="B699" s="0" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C699" s="0" t="s">
         <v>2</v>
@@ -10018,7 +10017,7 @@
         <v>9</v>
       </c>
       <c r="B700" s="0" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C700" s="0" t="s">
         <v>2</v>
@@ -10029,7 +10028,7 @@
         <v>9</v>
       </c>
       <c r="B701" s="0" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="C701" s="0" t="s">
         <v>2</v>
@@ -10040,7 +10039,7 @@
         <v>9</v>
       </c>
       <c r="B702" s="0" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="C702" s="0" t="s">
         <v>2</v>
@@ -10051,13 +10050,13 @@
         <v>9</v>
       </c>
       <c r="B703" s="0" t="s">
+        <v>599</v>
+      </c>
+      <c r="C703" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D703" s="0" t="s">
         <v>600</v>
-      </c>
-      <c r="C703" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D703" s="0" t="s">
-        <v>601</v>
       </c>
     </row>
     <row r="704" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10065,7 +10064,7 @@
         <v>9</v>
       </c>
       <c r="B704" s="0" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="C704" s="0" t="s">
         <v>2</v>
@@ -10076,7 +10075,7 @@
         <v>9</v>
       </c>
       <c r="B705" s="0" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C705" s="0" t="s">
         <v>2</v>
@@ -10087,7 +10086,7 @@
         <v>9</v>
       </c>
       <c r="B706" s="0" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="C706" s="0" t="s">
         <v>2</v>
@@ -10098,13 +10097,13 @@
         <v>9</v>
       </c>
       <c r="B707" s="0" t="s">
+        <v>603</v>
+      </c>
+      <c r="C707" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D707" s="0" t="s">
         <v>604</v>
-      </c>
-      <c r="C707" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D707" s="0" t="s">
-        <v>605</v>
       </c>
     </row>
     <row r="708" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10112,13 +10111,13 @@
         <v>9</v>
       </c>
       <c r="B708" s="0" t="s">
+        <v>555</v>
+      </c>
+      <c r="C708" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D708" s="0" t="s">
         <v>556</v>
-      </c>
-      <c r="C708" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D708" s="0" t="s">
-        <v>557</v>
       </c>
     </row>
     <row r="709" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10126,13 +10125,13 @@
         <v>9</v>
       </c>
       <c r="B709" s="0" t="s">
+        <v>555</v>
+      </c>
+      <c r="C709" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D709" s="0" t="s">
         <v>556</v>
-      </c>
-      <c r="C709" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D709" s="0" t="s">
-        <v>557</v>
       </c>
     </row>
     <row r="710" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10140,13 +10139,13 @@
         <v>9</v>
       </c>
       <c r="B710" s="0" t="s">
+        <v>605</v>
+      </c>
+      <c r="C710" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D710" s="0" t="s">
         <v>606</v>
-      </c>
-      <c r="C710" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D710" s="0" t="s">
-        <v>607</v>
       </c>
     </row>
     <row r="711" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10154,13 +10153,13 @@
         <v>9</v>
       </c>
       <c r="B711" s="0" t="s">
+        <v>607</v>
+      </c>
+      <c r="C711" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D711" s="0" t="s">
         <v>608</v>
-      </c>
-      <c r="C711" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D711" s="0" t="s">
-        <v>609</v>
       </c>
     </row>
     <row r="712" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10168,13 +10167,13 @@
         <v>9</v>
       </c>
       <c r="B712" s="0" t="s">
+        <v>609</v>
+      </c>
+      <c r="C712" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D712" s="0" t="s">
         <v>610</v>
-      </c>
-      <c r="C712" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D712" s="0" t="s">
-        <v>611</v>
       </c>
     </row>
     <row r="713" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10182,13 +10181,13 @@
         <v>9</v>
       </c>
       <c r="B713" s="0" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="C713" s="0" t="s">
         <v>14</v>
       </c>
       <c r="D713" s="0" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="714" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10196,13 +10195,13 @@
         <v>9</v>
       </c>
       <c r="B714" s="0" t="s">
+        <v>612</v>
+      </c>
+      <c r="C714" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D714" s="0" t="s">
         <v>613</v>
-      </c>
-      <c r="C714" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D714" s="0" t="s">
-        <v>614</v>
       </c>
     </row>
     <row r="715" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10210,13 +10209,13 @@
         <v>9</v>
       </c>
       <c r="B715" s="0" t="s">
+        <v>614</v>
+      </c>
+      <c r="C715" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D715" s="0" t="s">
         <v>615</v>
-      </c>
-      <c r="C715" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D715" s="0" t="s">
-        <v>616</v>
       </c>
     </row>
     <row r="716" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10224,13 +10223,13 @@
         <v>9</v>
       </c>
       <c r="B716" s="0" t="s">
+        <v>616</v>
+      </c>
+      <c r="C716" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D716" s="0" t="s">
         <v>617</v>
-      </c>
-      <c r="C716" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D716" s="0" t="s">
-        <v>618</v>
       </c>
     </row>
     <row r="717" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10238,13 +10237,13 @@
         <v>9</v>
       </c>
       <c r="B717" s="0" t="s">
+        <v>618</v>
+      </c>
+      <c r="C717" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D717" s="0" t="s">
         <v>619</v>
-      </c>
-      <c r="C717" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D717" s="0" t="s">
-        <v>620</v>
       </c>
     </row>
     <row r="718" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10252,13 +10251,13 @@
         <v>9</v>
       </c>
       <c r="B718" s="0" t="s">
+        <v>620</v>
+      </c>
+      <c r="C718" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D718" s="0" t="s">
         <v>621</v>
-      </c>
-      <c r="C718" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D718" s="0" t="s">
-        <v>622</v>
       </c>
     </row>
     <row r="719" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10266,13 +10265,13 @@
         <v>9</v>
       </c>
       <c r="B719" s="0" t="s">
+        <v>622</v>
+      </c>
+      <c r="C719" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D719" s="0" t="s">
         <v>623</v>
-      </c>
-      <c r="C719" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D719" s="0" t="s">
-        <v>624</v>
       </c>
     </row>
     <row r="720" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10280,13 +10279,13 @@
         <v>9</v>
       </c>
       <c r="B720" s="0" t="s">
+        <v>624</v>
+      </c>
+      <c r="C720" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D720" s="0" t="s">
         <v>625</v>
-      </c>
-      <c r="C720" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D720" s="0" t="s">
-        <v>626</v>
       </c>
     </row>
     <row r="721" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10294,13 +10293,13 @@
         <v>9</v>
       </c>
       <c r="B721" s="0" t="s">
+        <v>626</v>
+      </c>
+      <c r="C721" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D721" s="0" t="s">
         <v>627</v>
-      </c>
-      <c r="C721" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D721" s="0" t="s">
-        <v>628</v>
       </c>
     </row>
     <row r="722" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10308,13 +10307,13 @@
         <v>9</v>
       </c>
       <c r="B722" s="0" t="s">
+        <v>509</v>
+      </c>
+      <c r="C722" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D722" s="0" t="s">
         <v>510</v>
-      </c>
-      <c r="C722" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D722" s="0" t="s">
-        <v>511</v>
       </c>
     </row>
     <row r="723" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10322,13 +10321,13 @@
         <v>9</v>
       </c>
       <c r="B723" s="0" t="s">
+        <v>628</v>
+      </c>
+      <c r="C723" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D723" s="0" t="s">
         <v>629</v>
-      </c>
-      <c r="C723" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D723" s="0" t="s">
-        <v>630</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrected path in main
</commit_message>
<xml_diff>
--- a/GEO_list.xlsx
+++ b/GEO_list.xlsx
@@ -18,7 +18,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1522" uniqueCount="630">
   <si>
-    <t>GSE2296</t>
+    <t>GSE1441</t>
   </si>
   <si>
     <t>0,0.1,0.5,1,2,2.5,4,5,6,7,9,10,13,20,30,50,59,109,150,241</t>
@@ -2040,7 +2040,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Cleaned up argument names of step functions.
</commit_message>
<xml_diff>
--- a/GEO_list.xlsx
+++ b/GEO_list.xlsx
@@ -18,7 +18,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1522" uniqueCount="630">
   <si>
-    <t>GSE59015</t>
+    <t>GSE52428</t>
   </si>
   <si>
     <t>0,0.1,0.5,1,2,2.5,4,5,6,7,9,10,13,20,30,50,59,109,150,241</t>
@@ -2040,7 +2040,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>